<commit_message>
ACH added Huber and Maur
</commit_message>
<xml_diff>
--- a/data/raw/ACH/ACH_Receivers.xlsx
+++ b/data/raw/ACH/ACH_Receivers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\ACH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E68FDD-CE99-4045-B385-EB9045138A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105A4402-E86A-4E04-899F-D13657F20AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31550" yWindow="2650" windowWidth="27570" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32640" yWindow="2880" windowWidth="31580" windowHeight="19470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="180">
   <si>
     <t>Vendor ID</t>
   </si>
@@ -561,6 +561,21 @@
   </si>
   <si>
     <t>000528201557</t>
+  </si>
+  <si>
+    <t>0190078120</t>
+  </si>
+  <si>
+    <t>Huber, Louis</t>
+  </si>
+  <si>
+    <t>Louis Huber</t>
+  </si>
+  <si>
+    <t>Maurer, Dr. Robert</t>
+  </si>
+  <si>
+    <t>Robert J. Maurer</t>
   </si>
 </sst>
 </file>
@@ -645,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -698,6 +713,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -981,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" zoomScale="205" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="205" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2120,6 +2147,49 @@
         <v>13</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="20">
+        <v>312270324</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="24">
+        <v>121000358</v>
+      </c>
+      <c r="D54" s="24">
+        <v>441910852</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>